<commit_message>
añadido mi nave, ya pensare en un nombre mas trade
</commit_message>
<xml_diff>
--- a/Documentos/DiseñoKometKevin.xlsx
+++ b/Documentos/DiseñoKometKevin.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramiro\Downloads\PS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neblis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40041BDF-42FA-4234-BB11-9514F70536EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="26083" windowHeight="10868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Naves" sheetId="2" r:id="rId1"/>
     <sheet name="Asteroides" sheetId="3" r:id="rId2"/>
     <sheet name="Mejoras" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="67">
   <si>
     <t>Q</t>
   </si>
@@ -194,12 +200,45 @@
   </si>
   <si>
     <t>Escudo</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>Rayos laser del cañon derecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bomba que explota cuando dejas pretado el boton derecho </t>
+  </si>
+  <si>
+    <t>alto AOE pero baja cadencia</t>
+  </si>
+  <si>
+    <t>teleporte a corta distancia</t>
+  </si>
+  <si>
+    <t>semiautomatico cadencia media</t>
+  </si>
+  <si>
+    <t>muy alto</t>
+  </si>
+  <si>
+    <t>modo ''demonio'' que te have invencible y te quita los cooldowns durante un tiempo corto</t>
+  </si>
+  <si>
+    <t>bajo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -751,20 +790,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R82"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="10" max="10" width="3.125" customWidth="1"/>
+    <col min="11" max="11" width="12.125" customWidth="1"/>
+    <col min="18" max="18" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
@@ -1326,7 +1365,9 @@
       <c r="C26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
       <c r="G26" s="1"/>
@@ -1336,7 +1377,9 @@
       <c r="K26" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="L26" s="25"/>
+      <c r="L26" s="25" t="s">
+        <v>58</v>
+      </c>
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
       <c r="O26" s="1"/>
@@ -1349,7 +1392,9 @@
       <c r="C27" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="32" t="s">
+        <v>57</v>
+      </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -1359,7 +1404,9 @@
       <c r="K27" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="13"/>
+      <c r="L27" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -1382,7 +1429,9 @@
       <c r="K28" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L28" s="26"/>
+      <c r="L28" s="26" t="s">
+        <v>57</v>
+      </c>
       <c r="M28" s="26"/>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
@@ -1437,7 +1486,9 @@
       <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1449,7 +1500,9 @@
       <c r="K31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1514,7 +1567,9 @@
       <c r="C34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1526,7 +1581,9 @@
       <c r="K34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L34" s="15"/>
+      <c r="L34" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
@@ -1602,7 +1659,9 @@
       <c r="C38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1614,7 +1673,9 @@
       <c r="K38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L38" s="1"/>
+      <c r="L38" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -1629,7 +1690,9 @@
       <c r="C39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="11"/>
+      <c r="D39" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -1639,7 +1702,9 @@
       <c r="K39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L39" s="11"/>
+      <c r="L39" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
       <c r="O39" s="11"/>
@@ -1652,7 +1717,9 @@
       <c r="C40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -1664,7 +1731,9 @@
       <c r="K40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L40" s="11"/>
+      <c r="L40" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="M40" s="11"/>
       <c r="N40" s="11"/>
       <c r="O40" s="11"/>
@@ -2669,16 +2738,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -2873,14 +2942,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">

</xml_diff>